<commit_message>
Update to 2023.2 release.
Transferring 2023.2 release files from internal dev repo.
</commit_message>
<xml_diff>
--- a/quick_starts/qs4_transit/Data/inputs/Model_Parameters.xlsx
+++ b/quick_starts/qs4_transit/Data/inputs/Model_Parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\RDR\quick_starts\qs4_transit\Data\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F79D926D-D8B2-48CD-B9EA-8C475A3CBC8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E2F657C-A1E4-42ED-8878-4F0CE2136CBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30405" yWindow="1155" windowWidth="24750" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33780" yWindow="2715" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UncertaintyParameters" sheetId="1" r:id="rId1"/>
@@ -80,16 +80,16 @@
     <t>river flood, 10-year flood with no river level rise</t>
   </si>
   <si>
-    <t>Road_complete</t>
-  </si>
-  <si>
-    <t>Subway_complete</t>
-  </si>
-  <si>
     <t>haz</t>
   </si>
   <si>
     <t>01</t>
+  </si>
+  <si>
+    <t>Road</t>
+  </si>
+  <si>
+    <t>Rail</t>
   </si>
 </sst>
 </file>
@@ -449,7 +449,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -461,7 +461,7 @@
         <v>-1</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F2" s="2"/>
     </row>
@@ -533,7 +533,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -555,7 +557,7 @@
         <v>01</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -564,7 +566,7 @@
         <v>01</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -639,10 +641,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -663,6 +665,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="82817e06-30b9-43cf-b958-ceb9ef3b381f" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f48c015b-9737-41c0-a66b-fb1abee3a169">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -671,7 +684,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010027EA00A048AC0D429A85C51A62FECD2D" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="80f7edf319700d646fd7609c44aa8e05">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f48c015b-9737-41c0-a66b-fb1abee3a169" xmlns:ns3="82817e06-30b9-43cf-b958-ceb9ef3b381f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="02abb370397e3fd482f270da433270a9" ns2:_="" ns3:_="">
     <xsd:import namespace="f48c015b-9737-41c0-a66b-fb1abee3a169"/>
@@ -908,18 +921,18 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="82817e06-30b9-43cf-b958-ceb9ef3b381f" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f48c015b-9737-41c0-a66b-fb1abee3a169">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE52BB5C-9358-441E-A410-7A969818B080}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="82817e06-30b9-43cf-b958-ceb9ef3b381f"/>
+    <ds:schemaRef ds:uri="f48c015b-9737-41c0-a66b-fb1abee3a169"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD8F6EF4-D92D-492F-8846-64DCFBD977B9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -927,7 +940,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B585122-C183-441C-87FB-12422D5CCDBE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -944,15 +957,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE52BB5C-9358-441E-A410-7A969818B080}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="82817e06-30b9-43cf-b958-ceb9ef3b381f"/>
-    <ds:schemaRef ds:uri="f48c015b-9737-41c0-a66b-fb1abee3a169"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>